<commit_message>
Wrangled subjects properly, changed notes referring to incorrect name
</commit_message>
<xml_diff>
--- a/mss0048/OLR/xls_standard_input_MSS0048.xlsx
+++ b/mss0048/OLR/xls_standard_input_MSS0048.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\small_manuscript_collections\mss0048\Working_metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\domm-metadata\mss0048\OLR\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -133,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="717">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="721">
   <si>
     <t>text</t>
   </si>
@@ -2262,28 +2262,40 @@
     <t>1898-12-31</t>
   </si>
   <si>
-    <t>Letters from Conrad Wise Chapman to John Litton Chapman</t>
-  </si>
-  <si>
     <t>Chapman, Conrad Wise, 1842-1910</t>
   </si>
   <si>
-    <t>Chapman, John Litton</t>
-  </si>
-  <si>
     <t>Includes a document in Italian, a partial transcription from John Smith's The Generall Historie of Virginia, New-England, and the Summer Isles, The fovrth Booke, and an inventory of the estate of Thomas Chapman.</t>
   </si>
   <si>
-    <t>American Civil War (1861-1865)|Confederate States of America. Army</t>
-  </si>
-  <si>
     <t>Assorted letters from peers and associates. Items of interest include: an 1833 letter describing the ruins of General George Washington's childhood home in Fredericksburg, VA, including a sketch of the dwelling (presumably Ferry Farm); an 1833 letter discussing the sale of a slave family (the slave Syphax, accused of an unidentified transgression, and his wife and son) to the Chapmans; and a letter from the joint committee of Congress tasked to appoint artists to decorate the rotunda of the United States Capitol in Washington, D.C.</t>
   </si>
   <si>
-    <t>Washington, George, 1732-1799 -- Homes and haunts -- Virginia</t>
-  </si>
-  <si>
-    <t>United States Capitol (Washington, D.C.)|Slave trade -- West Virginia</t>
+    <t>Letters from Conrad Wise Chapman to John Linton Chapman</t>
+  </si>
+  <si>
+    <t>Chapman, John Linton</t>
+  </si>
+  <si>
+    <t>Presidents--Homes and haunts</t>
+  </si>
+  <si>
+    <t>Washington, George, 1732-1799</t>
+  </si>
+  <si>
+    <t>Virginia | West Virginia</t>
+  </si>
+  <si>
+    <t>United States Capitol (Washington, D.C.)</t>
+  </si>
+  <si>
+    <t>Slave trade</t>
+  </si>
+  <si>
+    <t>Confederate States of America. Army</t>
+  </si>
+  <si>
+    <t>American Civil War (1861-1865)</t>
   </si>
 </sst>
 </file>
@@ -3358,12 +3370,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V11"/>
+  <dimension ref="A1:W11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="O16" sqref="O16"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3377,22 +3389,23 @@
     <col min="7" max="7" width="16" style="21" customWidth="1"/>
     <col min="8" max="8" width="22" style="21" customWidth="1"/>
     <col min="9" max="9" width="75" style="21" customWidth="1"/>
-    <col min="10" max="11" width="23" style="21" customWidth="1"/>
+    <col min="10" max="10" width="31.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="37.28515625" style="21" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="23.28515625" style="21" customWidth="1"/>
     <col min="13" max="13" width="14.85546875" style="21" customWidth="1"/>
     <col min="14" max="14" width="15.140625" style="21" customWidth="1"/>
-    <col min="15" max="15" width="68.7109375" style="21" customWidth="1"/>
+    <col min="15" max="15" width="80.28515625" style="21" customWidth="1"/>
     <col min="16" max="16" width="67.140625" style="21" customWidth="1"/>
-    <col min="17" max="17" width="41.5703125" style="21" customWidth="1"/>
-    <col min="18" max="18" width="39.140625" style="21" customWidth="1"/>
-    <col min="19" max="19" width="13.42578125" style="21" customWidth="1"/>
-    <col min="20" max="20" width="42.85546875" style="21" customWidth="1"/>
-    <col min="21" max="21" width="56.140625" style="21" customWidth="1"/>
-    <col min="22" max="22" width="23.85546875" style="21" customWidth="1"/>
-    <col min="23" max="16384" width="9.140625" style="5"/>
+    <col min="17" max="17" width="39.140625" style="21" customWidth="1"/>
+    <col min="18" max="18" width="15.140625" style="21" customWidth="1"/>
+    <col min="19" max="19" width="59.85546875" style="21" customWidth="1"/>
+    <col min="20" max="20" width="64.7109375" style="21" customWidth="1"/>
+    <col min="21" max="22" width="56.140625" style="21" customWidth="1"/>
+    <col min="23" max="23" width="23.85546875" style="21" customWidth="1"/>
+    <col min="24" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="20" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" s="20" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>338</v>
       </c>
@@ -3442,25 +3455,28 @@
         <v>339</v>
       </c>
       <c r="Q1" s="19" t="s">
-        <v>343</v>
+        <v>352</v>
       </c>
       <c r="R1" s="19" t="s">
-        <v>352</v>
+        <v>15</v>
       </c>
       <c r="S1" s="19" t="s">
-        <v>15</v>
+        <v>459</v>
       </c>
       <c r="T1" s="19" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="U1" s="19" t="s">
         <v>460</v>
       </c>
       <c r="V1" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="W1" s="19" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>633</v>
       </c>
@@ -3501,25 +3517,34 @@
         <v>671</v>
       </c>
       <c r="O2" s="21" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
       <c r="P2" s="21" t="s">
         <v>672</v>
       </c>
+      <c r="Q2" s="21" t="s">
+        <v>673</v>
+      </c>
       <c r="R2" s="21" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="S2" s="21" t="s">
-        <v>674</v>
+        <v>715</v>
       </c>
       <c r="T2" s="21" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="U2" s="21" t="s">
+        <v>718</v>
+      </c>
+      <c r="V2" s="21" t="s">
+        <v>717</v>
+      </c>
+      <c r="W2" s="21" t="s">
         <v>716</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>634</v>
       </c>
@@ -3563,14 +3588,14 @@
       <c r="P3" s="21" t="s">
         <v>672</v>
       </c>
+      <c r="Q3" s="21" t="s">
+        <v>673</v>
+      </c>
       <c r="R3" s="21" t="s">
-        <v>673</v>
-      </c>
-      <c r="S3" s="21" t="s">
         <v>675</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>635</v>
       </c>
@@ -3619,14 +3644,14 @@
       <c r="P4" s="21" t="s">
         <v>672</v>
       </c>
+      <c r="Q4" s="21" t="s">
+        <v>673</v>
+      </c>
       <c r="R4" s="21" t="s">
-        <v>673</v>
-      </c>
-      <c r="S4" s="21" t="s">
         <v>676</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>636</v>
       </c>
@@ -3655,7 +3680,7 @@
         <v>692</v>
       </c>
       <c r="J5" s="21" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="K5" s="21" t="s">
         <v>667</v>
@@ -3672,17 +3697,20 @@
       <c r="P5" s="21" t="s">
         <v>672</v>
       </c>
+      <c r="Q5" s="21" t="s">
+        <v>673</v>
+      </c>
       <c r="R5" s="21" t="s">
-        <v>673</v>
-      </c>
-      <c r="S5" s="21" t="s">
         <v>677</v>
       </c>
-      <c r="U5" s="21" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="T5" s="21" t="s">
+        <v>720</v>
+      </c>
+      <c r="V5" s="21" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>637</v>
       </c>
@@ -3711,7 +3739,7 @@
         <v>692</v>
       </c>
       <c r="J6" s="21" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="K6" s="21" t="s">
         <v>667</v>
@@ -3728,17 +3756,20 @@
       <c r="P6" s="21" t="s">
         <v>672</v>
       </c>
+      <c r="Q6" s="21" t="s">
+        <v>673</v>
+      </c>
       <c r="R6" s="21" t="s">
-        <v>673</v>
-      </c>
-      <c r="S6" s="21" t="s">
         <v>678</v>
       </c>
-      <c r="U6" s="21" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="T6" s="21" t="s">
+        <v>720</v>
+      </c>
+      <c r="V6" s="21" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>638</v>
       </c>
@@ -3767,7 +3798,7 @@
         <v>692</v>
       </c>
       <c r="J7" s="21" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="K7" s="21" t="s">
         <v>667</v>
@@ -3784,17 +3815,20 @@
       <c r="P7" s="21" t="s">
         <v>672</v>
       </c>
+      <c r="Q7" s="21" t="s">
+        <v>673</v>
+      </c>
       <c r="R7" s="21" t="s">
-        <v>673</v>
-      </c>
-      <c r="S7" s="21" t="s">
         <v>679</v>
       </c>
-      <c r="U7" s="21" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="T7" s="21" t="s">
+        <v>720</v>
+      </c>
+      <c r="V7" s="21" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
         <v>639</v>
       </c>
@@ -3823,7 +3857,7 @@
         <v>692</v>
       </c>
       <c r="J8" s="21" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="K8" s="21" t="s">
         <v>667</v>
@@ -3840,17 +3874,20 @@
       <c r="P8" s="21" t="s">
         <v>672</v>
       </c>
+      <c r="Q8" s="21" t="s">
+        <v>673</v>
+      </c>
       <c r="R8" s="21" t="s">
-        <v>673</v>
-      </c>
-      <c r="S8" s="21" t="s">
         <v>680</v>
       </c>
-      <c r="U8" s="21" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="T8" s="21" t="s">
+        <v>720</v>
+      </c>
+      <c r="V8" s="21" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>640</v>
       </c>
@@ -3879,7 +3916,7 @@
         <v>696</v>
       </c>
       <c r="J9" s="21" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="K9" s="21" t="s">
         <v>667</v>
@@ -3897,17 +3934,20 @@
       <c r="P9" s="21" t="s">
         <v>672</v>
       </c>
+      <c r="Q9" s="21" t="s">
+        <v>673</v>
+      </c>
       <c r="R9" s="21" t="s">
-        <v>673</v>
-      </c>
-      <c r="S9" s="21" t="s">
         <v>681</v>
       </c>
-      <c r="U9" s="21" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="T9" s="21" t="s">
+        <v>720</v>
+      </c>
+      <c r="V9" s="21" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
         <v>641</v>
       </c>
@@ -3933,13 +3973,13 @@
         <v>358</v>
       </c>
       <c r="I10" s="21" t="s">
+        <v>712</v>
+      </c>
+      <c r="J10" s="21" t="s">
         <v>709</v>
       </c>
-      <c r="J10" s="21" t="s">
-        <v>710</v>
-      </c>
       <c r="K10" s="21" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
       <c r="L10" s="21" t="s">
         <v>706</v>
@@ -3953,14 +3993,14 @@
       <c r="P10" s="21" t="s">
         <v>672</v>
       </c>
+      <c r="Q10" s="21" t="s">
+        <v>673</v>
+      </c>
       <c r="R10" s="21" t="s">
-        <v>673</v>
-      </c>
-      <c r="S10" s="21" t="s">
         <v>682</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>642</v>
       </c>
@@ -3998,15 +4038,15 @@
         <v>703</v>
       </c>
       <c r="O11" s="22" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="P11" s="21" t="s">
         <v>672</v>
       </c>
+      <c r="Q11" s="21" t="s">
+        <v>673</v>
+      </c>
       <c r="R11" s="21" t="s">
-        <v>673</v>
-      </c>
-      <c r="S11" s="21" t="s">
         <v>683</v>
       </c>
     </row>
@@ -4060,7 +4100,7 @@
           <x14:formula1>
             <xm:f>'Select-a-header values'!$G$1:$G$17</xm:f>
           </x14:formula1>
-          <xm:sqref>T1:V1</xm:sqref>
+          <xm:sqref>S1:W1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
@@ -4070,15 +4110,9 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
-            <xm:f>'Select-a-header values'!$E$1:$E$34</xm:f>
-          </x14:formula1>
-          <xm:sqref>O1:R1</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
-          <x14:formula1>
             <xm:f>'Select-a-header values'!$F$1:$F$21</xm:f>
           </x14:formula1>
-          <xm:sqref>S1</xm:sqref>
+          <xm:sqref>R1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="Please choose a value from the dropdown list" prompt="Please choose a value from the dropdown list">
           <x14:formula1>
@@ -4097,6 +4131,12 @@
             <xm:f>'CV values'!$D$2:$D$60</xm:f>
           </x14:formula1>
           <xm:sqref>H2:H1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
+          <x14:formula1>
+            <xm:f>'Select-a-header values'!$E$1:$E$34</xm:f>
+          </x14:formula1>
+          <xm:sqref>O1:Q1</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -6526,7 +6566,7 @@
   <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Incorporated Laurel's changes to a note
</commit_message>
<xml_diff>
--- a/mss0048/OLR/xls_standard_input_MSS0048.xlsx
+++ b/mss0048/OLR/xls_standard_input_MSS0048.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\domm-metadata\mss0048\OLR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\small_manuscript_collections\mss0048\Final_metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2268,9 +2268,6 @@
     <t>Includes a document in Italian, a partial transcription from John Smith's The Generall Historie of Virginia, New-England, and the Summer Isles, The fovrth Booke, and an inventory of the estate of Thomas Chapman.</t>
   </si>
   <si>
-    <t>Assorted letters from peers and associates. Items of interest include: an 1833 letter describing the ruins of General George Washington's childhood home in Fredericksburg, VA, including a sketch of the dwelling (presumably Ferry Farm); an 1833 letter discussing the sale of a slave family (the slave Syphax, accused of an unidentified transgression, and his wife and son) to the Chapmans; and a letter from the joint committee of Congress tasked to appoint artists to decorate the rotunda of the United States Capitol in Washington, D.C.</t>
-  </si>
-  <si>
     <t>Letters from Conrad Wise Chapman to John Linton Chapman</t>
   </si>
   <si>
@@ -2296,6 +2293,9 @@
   </si>
   <si>
     <t>American Civil War (1861-1865)</t>
+  </si>
+  <si>
+    <t>Assorted letters from peers and associates. Items of interest include: an 1833 letter describing the ruins of General George Washington's childhood home in Fredericksburg, VA, including a sketch of the dwelling (presumably Ferry Farm); an 1833 letter discussing the sale of a slave family (the slave Syphax, accused of an unidentified transgression, and his wife and son) from Jane Washington at Claymont Court to the Chapmans; and a letter from the joint committee of Congress tasked to appoint artists to decorate the rotunda of the United States Capitol in Washington, D.C.</t>
   </si>
 </sst>
 </file>
@@ -3375,7 +3375,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomLeft" activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3517,7 +3517,7 @@
         <v>671</v>
       </c>
       <c r="O2" s="21" t="s">
-        <v>711</v>
+        <v>720</v>
       </c>
       <c r="P2" s="21" t="s">
         <v>672</v>
@@ -3529,19 +3529,19 @@
         <v>674</v>
       </c>
       <c r="S2" s="21" t="s">
+        <v>714</v>
+      </c>
+      <c r="T2" s="21" t="s">
+        <v>713</v>
+      </c>
+      <c r="U2" s="21" t="s">
+        <v>717</v>
+      </c>
+      <c r="V2" s="21" t="s">
+        <v>716</v>
+      </c>
+      <c r="W2" s="21" t="s">
         <v>715</v>
-      </c>
-      <c r="T2" s="21" t="s">
-        <v>714</v>
-      </c>
-      <c r="U2" s="21" t="s">
-        <v>718</v>
-      </c>
-      <c r="V2" s="21" t="s">
-        <v>717</v>
-      </c>
-      <c r="W2" s="21" t="s">
-        <v>716</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
@@ -3704,10 +3704,10 @@
         <v>677</v>
       </c>
       <c r="T5" s="21" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="V5" s="21" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
@@ -3763,10 +3763,10 @@
         <v>678</v>
       </c>
       <c r="T6" s="21" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="V6" s="21" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
@@ -3822,10 +3822,10 @@
         <v>679</v>
       </c>
       <c r="T7" s="21" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="V7" s="21" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
@@ -3881,10 +3881,10 @@
         <v>680</v>
       </c>
       <c r="T8" s="21" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="V8" s="21" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
@@ -3941,10 +3941,10 @@
         <v>681</v>
       </c>
       <c r="T9" s="21" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="V9" s="21" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
@@ -3973,13 +3973,13 @@
         <v>358</v>
       </c>
       <c r="I10" s="21" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="J10" s="21" t="s">
         <v>709</v>
       </c>
       <c r="K10" s="21" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="L10" s="21" t="s">
         <v>706</v>

</xml_diff>

<commit_message>
Finalized wrangling for prod ingest, added missing subject:person
</commit_message>
<xml_diff>
--- a/mss0048/OLR/xls_standard_input_MSS0048.xlsx
+++ b/mss0048/OLR/xls_standard_input_MSS0048.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\small_manuscript_collections\mss0048\Final_metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\domm-metadata\mss0048\OLR\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -133,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="721">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="721">
   <si>
     <t>text</t>
   </si>
@@ -3372,10 +3372,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="O24" sqref="O24"/>
+      <selection pane="bottomLeft" activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3649,6 +3649,9 @@
       </c>
       <c r="R4" s="21" t="s">
         <v>676</v>
+      </c>
+      <c r="S4" s="21" t="s">
+        <v>684</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">

</xml_diff>